<commit_message>
Update spreadsheet color coding
</commit_message>
<xml_diff>
--- a/LMETutorialScripts/LME_EventMarkerMappingKey.xlsx
+++ b/LMETutorialScripts/LME_EventMarkerMappingKey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projects\InProgress\LME_MixedEffectsERPTutorial\Data\LME_04_TutorialCode\Tutorial_01_MATLAB_EEGProcessing\FilesUsedForDataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854A664D-AD47-4CC4-B46A-50884AB54864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434CCF3C-37EB-438C-B823-36EECE462BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="16220" windowHeight="8620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,39 +253,16 @@
     <t xml:space="preserve">This spreadsheet lists the mappings between original event markers (listed in the raw data file) and the 3-digit preceding codes (flags composed of an emotion condition ID and actor ID). </t>
   </si>
   <si>
-    <t xml:space="preserve">3-digit preceding code composed of the emotion condition and actor ID. The first digit of the preceding code is the same as the EmotionCode column (e.g., 301 is a stimulus with emotion condition of 3). The last two digits of the preceding code is the same as the ActorCode column (e.g., 301 is a stimulus with actor ID of 01). </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">NOTE: In </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LME_01_AddUniqueFlags.m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, the 3-digit preceding code is combined with a presentation number (ranging from 01-10) to create the final 5-digit event marker. For example, 30101 is the first presentation of the Angry emotion/actor ID 01 stimulus. </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Actor ID used in the unique preceding codes. There are 5 actor IDs in this example: 01, 02, 03, 04, 05. </t>
   </si>
   <si>
     <t xml:space="preserve">This file contains one sheet, corresponding to 1 experiment condition (Experiment1). If your experiment is not fully crossed  (e.g., subjects were assigned different actors in order to match the subject’s own race), you may need additional sheets for specifying each set of event markers.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">These scripts extract the 3-digit preceding code and combine it with a presentation number (ranging from 01-10) to create the final 5-digit event marker. For example, 30101 is the first presentation of the Angry emotion/actor ID 01 stimulus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-digit preceding code composed of the emotion condition and actor IDs. The first digit of the preceding code is the same as the EmotionCode column (e.g., 301 is a stimulus with emotion condition of 3). The last two digits of the preceding code is the same as the ActorCode column (e.g., 301 is a stimulus with actor ID of 01). </t>
   </si>
 </sst>
 </file>
@@ -380,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -392,9 +369,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,9 +665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBC99BA-34D5-4D31-BE67-642C7B5CCF0B}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -699,105 +686,104 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -812,7 +798,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,16 +814,16 @@
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="21" t="s">
         <v>25</v>
       </c>
     </row>
@@ -848,16 +834,16 @@
       <c r="B2" s="3">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="14">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="15">
         <v>301</v>
       </c>
     </row>
@@ -868,16 +854,16 @@
       <c r="B3" s="3">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="14">
         <v>2</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="15">
         <v>302</v>
       </c>
     </row>
@@ -888,16 +874,16 @@
       <c r="B4" s="3">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="14">
         <v>3</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="15">
         <v>303</v>
       </c>
     </row>
@@ -908,16 +894,16 @@
       <c r="B5" s="3">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="14">
         <v>4</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="15">
         <v>304</v>
       </c>
     </row>
@@ -928,16 +914,16 @@
       <c r="B6" s="3">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="14">
         <v>5</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="15">
         <v>305</v>
       </c>
     </row>
@@ -948,16 +934,16 @@
       <c r="B7" s="4">
         <v>90</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>5</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="12">
         <v>1</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="13">
         <v>501</v>
       </c>
     </row>
@@ -968,16 +954,16 @@
       <c r="B8" s="4">
         <v>91</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="12">
         <v>2</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="13">
         <v>502</v>
       </c>
     </row>
@@ -988,16 +974,16 @@
       <c r="B9" s="4">
         <v>92</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="12">
         <v>3</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="13">
         <v>503</v>
       </c>
     </row>
@@ -1008,16 +994,16 @@
       <c r="B10" s="4">
         <v>93</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="12">
         <v>4</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="13">
         <v>504</v>
       </c>
     </row>
@@ -1028,16 +1014,16 @@
       <c r="B11" s="4">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="12">
         <v>5</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="13">
         <v>505</v>
       </c>
     </row>
@@ -1048,16 +1034,16 @@
       <c r="B12" s="5">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>6</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="16">
         <v>1</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="17">
         <v>601</v>
       </c>
     </row>
@@ -1068,16 +1054,16 @@
       <c r="B13" s="5">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>6</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="16">
         <v>2</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="17">
         <v>602</v>
       </c>
     </row>
@@ -1088,16 +1074,16 @@
       <c r="B14" s="5">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>6</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="16">
         <v>3</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="17">
         <v>603</v>
       </c>
     </row>
@@ -1108,16 +1094,16 @@
       <c r="B15" s="5">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>6</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="16">
         <v>4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="17">
         <v>604</v>
       </c>
     </row>
@@ -1128,16 +1114,16 @@
       <c r="B16" s="5">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>6</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="16">
         <v>5</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="17">
         <v>605</v>
       </c>
     </row>
@@ -1148,16 +1134,16 @@
       <c r="B17" s="6">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>8</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="18">
         <v>1</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="19">
         <v>801</v>
       </c>
     </row>
@@ -1168,16 +1154,16 @@
       <c r="B18" s="6">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>8</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="18">
         <v>2</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="19">
         <v>802</v>
       </c>
     </row>
@@ -1188,16 +1174,16 @@
       <c r="B19" s="6">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>8</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="18">
         <v>3</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="19">
         <v>803</v>
       </c>
     </row>
@@ -1208,16 +1194,16 @@
       <c r="B20" s="6">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>8</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="18">
         <v>4</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="19">
         <v>804</v>
       </c>
     </row>
@@ -1228,21 +1214,21 @@
       <c r="B21" s="6">
         <v>24</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>8</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="18">
         <v>5</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="19">
         <v>805</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update spreadsheet Key sheet
</commit_message>
<xml_diff>
--- a/LMETutorialScripts/LME_EventMarkerMappingKey.xlsx
+++ b/LMETutorialScripts/LME_EventMarkerMappingKey.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projects\InProgress\LME_MixedEffectsERPTutorial\Data\LME_04_TutorialCode\Tutorial_01_MATLAB_EEGProcessing\FilesUsedForDataProcessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projects\InProgress\LME_MixedEffectsERPTutorial\Data\LME_04_GitHubTutorialCode\Tutorial_01_MATLAB_EEGProcessing\FilesUsedForDataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434CCF3C-37EB-438C-B823-36EECE462BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="16220" windowHeight="8620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28650" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="5" r:id="rId1"/>
     <sheet name="Experiment1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -256,19 +255,19 @@
     <t xml:space="preserve">Actor ID used in the unique preceding codes. There are 5 actor IDs in this example: 01, 02, 03, 04, 05. </t>
   </si>
   <si>
-    <t xml:space="preserve">This file contains one sheet, corresponding to 1 experiment condition (Experiment1). If your experiment is not fully crossed  (e.g., subjects were assigned different actors in order to match the subject’s own race), you may need additional sheets for specifying each set of event markers.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">These scripts extract the 3-digit preceding code and combine it with a presentation number (ranging from 01-10) to create the final 5-digit event marker. For example, 30101 is the first presentation of the Angry emotion/actor ID 01 stimulus. </t>
   </si>
   <si>
     <t xml:space="preserve">3-digit preceding code composed of the emotion condition and actor IDs. The first digit of the preceding code is the same as the EmotionCode column (e.g., 301 is a stimulus with emotion condition of 3). The last two digits of the preceding code is the same as the ActorCode column (e.g., 301 is a stimulus with actor ID of 01). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This file contains one sheet, corresponding to 1 experiment condition (Experiment1). If your experiment design is not fully crossed  (e.g., subjects were assigned different actors in order to match the subject’s own race), you may need additional sheets for specifying each set of event markers.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00"/>
     <numFmt numFmtId="165" formatCode="000"/>
@@ -664,64 +663,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBC99BA-34D5-4D31-BE67-642C7B5CCF0B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
@@ -729,7 +728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
@@ -737,7 +736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>28</v>
       </c>
@@ -745,7 +744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
@@ -753,7 +752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>39</v>
       </c>
@@ -761,28 +760,28 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>37</v>
       </c>
@@ -794,20 +793,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.90625" style="1"/>
-    <col min="6" max="6" width="20.1796875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1"/>
+    <col min="6" max="6" width="20.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -827,7 +826,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -847,7 +846,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -867,7 +866,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -887,7 +886,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -907,7 +906,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -927,7 +926,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -947,7 +946,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -967,7 +966,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -987,7 +986,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1027,7 +1026,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>21</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>24</v>
       </c>

</xml_diff>